<commit_message>
fixed error on linux, random() was already defined
chaged random() to randomNum()
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\USF and education\spring 2020\Operating Systems\Project 2 paging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CEDE23-DB57-468D-9521-30467577C95B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5259432E-5848-4441-BD78-D38E3A085475}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13968" yWindow="516" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1176" yWindow="2280" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,7 +394,7 @@
     <col min="3" max="3" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -408,7 +408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -431,305 +431,631 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>999723</v>
+      </c>
+      <c r="C3">
+        <v>122343</v>
+      </c>
+      <c r="D3">
+        <v>228838</v>
+      </c>
+      <c r="E3">
+        <v>54321</v>
+      </c>
+      <c r="F3">
+        <v>154429</v>
+      </c>
+      <c r="G3">
+        <v>44024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>627141</v>
+      </c>
+      <c r="C4">
+        <v>118010</v>
+      </c>
+      <c r="D4">
+        <v>128601</v>
+      </c>
+      <c r="E4">
+        <v>38644</v>
+      </c>
+      <c r="F4">
+        <v>92770</v>
+      </c>
+      <c r="G4">
+        <v>35650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>626068</v>
+      </c>
+      <c r="C5">
+        <v>117824</v>
+      </c>
+      <c r="D5">
+        <v>47828</v>
+      </c>
+      <c r="E5">
+        <v>18797</v>
+      </c>
+      <c r="F5">
+        <v>30691</v>
+      </c>
+      <c r="G5">
+        <v>11092</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>625223</v>
+      </c>
+      <c r="C6">
+        <v>117688</v>
+      </c>
+      <c r="D6">
+        <v>3820</v>
+      </c>
+      <c r="E6">
+        <v>1335</v>
+      </c>
+      <c r="F6">
+        <v>3344</v>
+      </c>
+      <c r="G6">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>617110</v>
+      </c>
+      <c r="C7">
+        <v>116175</v>
+      </c>
+      <c r="D7">
+        <v>2497</v>
+      </c>
+      <c r="E7">
+        <v>851</v>
+      </c>
+      <c r="F7">
+        <v>2133</v>
+      </c>
+      <c r="G7">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="B8">
+        <v>550472</v>
+      </c>
+      <c r="C8">
+        <v>102596</v>
+      </c>
+      <c r="D8">
+        <v>1467</v>
+      </c>
+      <c r="E8">
+        <v>514</v>
+      </c>
+      <c r="F8">
+        <v>1264</v>
+      </c>
+      <c r="G8">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>128</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="B9">
+        <v>473343</v>
+      </c>
+      <c r="C9">
+        <v>83342</v>
+      </c>
+      <c r="D9">
+        <v>891</v>
+      </c>
+      <c r="E9">
+        <v>305</v>
+      </c>
+      <c r="F9">
+        <v>771</v>
+      </c>
+      <c r="G9">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>256</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="B10">
+        <v>132105</v>
+      </c>
+      <c r="C10">
+        <v>13277</v>
+      </c>
+      <c r="D10">
+        <v>511</v>
+      </c>
+      <c r="E10">
+        <v>125</v>
+      </c>
+      <c r="F10">
+        <v>397</v>
+      </c>
+      <c r="G10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>512</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="B11">
+        <v>316</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>317</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>317</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>1024</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B12">
+        <v>316</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>317</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>317</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>1</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>4</v>
+      <c r="B16">
+        <v>999700</v>
+      </c>
+      <c r="C16">
+        <v>107180</v>
+      </c>
+      <c r="D16">
+        <v>460912</v>
+      </c>
+      <c r="E16">
+        <v>76432</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>715743</v>
+      </c>
+      <c r="C17">
+        <v>104907</v>
+      </c>
+      <c r="D17">
+        <v>302860</v>
+      </c>
+      <c r="E17">
+        <v>55013</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>715721</v>
+      </c>
+      <c r="C18">
+        <v>104894</v>
+      </c>
+      <c r="D18">
+        <v>205368</v>
+      </c>
+      <c r="E18">
+        <v>37524</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>64</v>
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>702468</v>
+      </c>
+      <c r="C19">
+        <v>101870</v>
+      </c>
+      <c r="D19">
+        <v>138539</v>
+      </c>
+      <c r="E19">
+        <v>24043</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>128</v>
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>634403</v>
+      </c>
+      <c r="C20">
+        <v>95235</v>
+      </c>
+      <c r="D20">
+        <v>98067</v>
+      </c>
+      <c r="E20">
+        <v>16759</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>256</v>
+        <v>64</v>
+      </c>
+      <c r="B21">
+        <v>447146</v>
+      </c>
+      <c r="C21">
+        <v>40508</v>
+      </c>
+      <c r="D21">
+        <v>70315</v>
+      </c>
+      <c r="E21">
+        <v>12053</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>512</v>
+        <v>128</v>
+      </c>
+      <c r="B22">
+        <v>420733</v>
+      </c>
+      <c r="C22">
+        <v>36159</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
+        <v>256</v>
+      </c>
+      <c r="B23">
+        <v>311520</v>
+      </c>
+      <c r="C23">
+        <v>26017</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>512</v>
+      </c>
+      <c r="B24">
+        <v>266155</v>
+      </c>
+      <c r="C24">
+        <v>20813</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>1024</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B25">
+        <v>64012</v>
+      </c>
+      <c r="C25">
+        <v>7732</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>8</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>0</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" t="s">
         <v>3</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F27" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>4</v>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>128</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>256</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>512</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>1024</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>7</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>0</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D40" t="s">
         <v>3</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F40" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>8</v>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>64</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>128</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>256</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>512</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
         <v>1024</v>
       </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
seg fault on linux related to fscanf, everything working correctly otherwise
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\USF and education\spring 2020\Operating Systems\Project 2 paging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8191A9C3-ED58-4D26-BA58-1BA6C2F37E4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC90A95-2F9F-4528-A526-17234DDF79D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1085,6 +1084,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>RDM</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1101,10 +1103,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1134,6 +1136,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1173,6 +1181,1273 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>64012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000028-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>RDM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$16:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>107180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>104907</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104894</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101870</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95235</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40508</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36159</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20813</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7732</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000029-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>FIFO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$16:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>460912</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>302860</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205368</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>138539</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>98067</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70315</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48526</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31698</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15609</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6673</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002B-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>FIFO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$16:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>76432</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37524</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24043</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16759</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12053</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8487</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5945</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3425</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1747</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002C-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>LRU</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$16:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>403955</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>243809</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>171186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116604</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59089</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25308</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10425</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4391</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002D-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>LRU</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$16:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>74158</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43187</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23983</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14749</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11737</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8863</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6131</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4231</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>955</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002E-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>VMS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$16:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>545640</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>388568</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>336525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>305768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>284110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>264663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>238586</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>215724</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>135154</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76523</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-F155-45BC-93ED-0F34C8C3C569}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>VMS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$16:$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>77389</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26954</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15909</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10489</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7225</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5122</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3257</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1028</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>427</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-F155-45BC-93ED-0F34C8C3C569}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="449709104"/>
+        <c:axId val="449718944"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="449709104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Frames</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="449718944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="449718944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Reads/Writes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="449709104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>swim.trace</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$53:$A$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$53:$B$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>525860</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>380532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>379940</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>320581</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>279574</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>270502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>196326</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170190</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150289</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>102178</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39292</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2542</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1203,10 +2478,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$53:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1236,45 +2511,57 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$25</c:f>
+              <c:f>Sheet1!$C$53:$C$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>107180</c:v>
+                  <c:v>67038</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>104907</c:v>
+                  <c:v>57518</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104894</c:v>
+                  <c:v>57379</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>101870</c:v>
+                  <c:v>56608</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95235</c:v>
+                  <c:v>56537</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40508</c:v>
+                  <c:v>55996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36159</c:v>
+                  <c:v>42275</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26017</c:v>
+                  <c:v>39202</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20813</c:v>
+                  <c:v>35338</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7732</c:v>
+                  <c:v>24794</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9988</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1303,10 +2590,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$53:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1336,45 +2623,57 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$25</c:f>
+              <c:f>Sheet1!$D$53:$D$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>460912</c:v>
+                  <c:v>541458</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>302860</c:v>
+                  <c:v>419509</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>205368</c:v>
+                  <c:v>330893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>138539</c:v>
+                  <c:v>214295</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98067</c:v>
+                  <c:v>81638</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70315</c:v>
+                  <c:v>30422</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48526</c:v>
+                  <c:v>17523</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31698</c:v>
+                  <c:v>8551</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15609</c:v>
+                  <c:v>4850</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6673</c:v>
+                  <c:v>3264</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2798</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2543</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1403,10 +2702,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$53:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1436,45 +2735,57 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$16:$E$25</c:f>
+              <c:f>Sheet1!$E$53:$E$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>76432</c:v>
+                  <c:v>60678</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55013</c:v>
+                  <c:v>57750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37524</c:v>
+                  <c:v>55488</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24043</c:v>
+                  <c:v>47434</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16759</c:v>
+                  <c:v>18172</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12053</c:v>
+                  <c:v>7585</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8487</c:v>
+                  <c:v>4932</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5945</c:v>
+                  <c:v>2836</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3425</c:v>
+                  <c:v>1624</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1747</c:v>
+                  <c:v>969</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1503,10 +2814,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$53:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1536,45 +2847,57 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$16:$F$25</c:f>
+              <c:f>Sheet1!$F$53:$F$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>403955</c:v>
+                  <c:v>470679</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>243809</c:v>
+                  <c:v>346936</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>171186</c:v>
+                  <c:v>285375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>116604</c:v>
+                  <c:v>171961</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84401</c:v>
+                  <c:v>48254</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59089</c:v>
+                  <c:v>21656</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40821</c:v>
+                  <c:v>13250</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25308</c:v>
+                  <c:v>5673</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10425</c:v>
+                  <c:v>3632</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4391</c:v>
+                  <c:v>2803</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2543</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1603,10 +2926,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$53:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1636,45 +2959,57 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$25</c:f>
+              <c:f>Sheet1!$G$53:$G$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>74158</c:v>
+                  <c:v>60029</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43187</c:v>
+                  <c:v>56045</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23983</c:v>
+                  <c:v>53614</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14749</c:v>
+                  <c:v>46293</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11737</c:v>
+                  <c:v>9674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8863</c:v>
+                  <c:v>5687</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6131</c:v>
+                  <c:v>3812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4231</c:v>
+                  <c:v>1866</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2173</c:v>
+                  <c:v>1159</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>955</c:v>
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1686,13 +3021,257 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="449709104"/>
+        <c:axId val="449718944"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="449709104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="449718944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="449718944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="600000.00000000012"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="449709104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>sixpack.trace</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1703,10 +3282,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$36:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1736,45 +3315,57 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$16:$H$25</c:f>
+              <c:f>Sheet1!$B$36:$B$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>545640</c:v>
+                  <c:v>999921</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>388568</c:v>
+                  <c:v>791209</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>336525</c:v>
+                  <c:v>791127</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>305768</c:v>
+                  <c:v>790793</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>284110</c:v>
+                  <c:v>788840</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>264663</c:v>
+                  <c:v>772374</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>238586</c:v>
+                  <c:v>722048</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>215724</c:v>
+                  <c:v>679876</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>135154</c:v>
+                  <c:v>628516</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76523</c:v>
+                  <c:v>552877</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119282</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1782,17 +3373,19 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-F155-45BC-93ED-0F34C8C3C569}"/>
+              <c16:uniqueId val="{00000028-5B9B-4405-AAAB-E16E65F752F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1803,10 +3396,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:f>Sheet1!$A$36:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1836,45 +3429,57 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$16:$I$25</c:f>
+              <c:f>Sheet1!$C$36:$C$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>77389</c:v>
+                  <c:v>160982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26954</c:v>
+                  <c:v>159398</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15909</c:v>
+                  <c:v>159395</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10489</c:v>
+                  <c:v>159145</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7225</c:v>
+                  <c:v>158922</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5122</c:v>
+                  <c:v>153941</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3257</c:v>
+                  <c:v>138438</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2015</c:v>
+                  <c:v>135514</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1028</c:v>
+                  <c:v>118656</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>427</c:v>
+                  <c:v>114185</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25756</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1882,7 +3487,455 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-F155-45BC-93ED-0F34C8C3C569}"/>
+              <c16:uniqueId val="{00000029-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$36:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$36:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>529237</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>351810</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230168</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140083</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85283</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27778</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15440</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8089</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5492</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4314</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3890</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002B-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$36:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$36:$E$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>136484</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94710</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57121</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31314</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18805</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11936</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8346</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5426</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3353</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2368</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1581</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002C-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$36:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$36:$F$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>483161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>282620</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>176496</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>108682</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67747</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41186</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21090</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11240</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5823</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4468</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3951</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3890</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002D-5B9B-4405-AAAB-E16E65F752F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$36:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$36:$G$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>135857</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71260</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32717</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19342</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13730</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9672</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6526</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4092</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2444</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1846</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1356</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002E-5B9B-4405-AAAB-E16E65F752F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2132,6 +4185,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3164,20 +5297,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3233,6 +6398,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B73CBF6D-8634-4ABD-85AA-C044BA28FA4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F4378F9-FC06-461A-B841-F3164368FF28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3754,19 +6991,529 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4472C4"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride3.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4472C4"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4372,6 +8119,64 @@
         <v>427</v>
       </c>
     </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>2048</v>
+      </c>
+      <c r="B26">
+        <v>13052</v>
+      </c>
+      <c r="C26">
+        <v>3452</v>
+      </c>
+      <c r="D26">
+        <v>3432</v>
+      </c>
+      <c r="E26">
+        <v>700</v>
+      </c>
+      <c r="F26">
+        <v>2904</v>
+      </c>
+      <c r="G26">
+        <v>427</v>
+      </c>
+      <c r="H26">
+        <v>3564</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>4096</v>
+      </c>
+      <c r="B27">
+        <v>2851</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>2852</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>2852</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>2852</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>8</v>
@@ -4639,6 +8444,52 @@
         <v>1846</v>
       </c>
     </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>2048</v>
+      </c>
+      <c r="B46">
+        <v>119282</v>
+      </c>
+      <c r="C46">
+        <v>25756</v>
+      </c>
+      <c r="D46">
+        <v>4314</v>
+      </c>
+      <c r="E46">
+        <v>1581</v>
+      </c>
+      <c r="F46">
+        <v>3951</v>
+      </c>
+      <c r="G46">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>4096</v>
+      </c>
+      <c r="B47">
+        <v>3889</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>3890</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>3890</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>7</v>
@@ -4907,13 +8758,54 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="2"/>
+      <c r="A63" s="2">
+        <v>2048</v>
+      </c>
+      <c r="B63">
+        <v>39292</v>
+      </c>
+      <c r="C63">
+        <v>9988</v>
+      </c>
+      <c r="D63">
+        <v>2798</v>
+      </c>
+      <c r="E63">
+        <v>350</v>
+      </c>
+      <c r="F63">
+        <v>2576</v>
+      </c>
+      <c r="G63">
+        <v>259</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="2"/>
+      <c r="A64" s="2">
+        <v>4096</v>
+      </c>
+      <c r="B64">
+        <v>2542</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>2543</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>2543</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>